<commit_message>
add case for multiple routing
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765DA86C-F857-43CF-B334-A4BDDE05A753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DCCF4D-A46B-4E6A-99B5-EBD1BDC42144}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
   <si>
     <t>name</t>
   </si>
@@ -286,6 +286,51 @@
   </si>
   <si>
     <t>id='6' AND org_name='苏州西门子有限公司'</t>
+  </si>
+  <si>
+    <t>iot-connector-oneDb</t>
+  </si>
+  <si>
+    <t>good request, data retrieved (no schema check)</t>
+  </si>
+  <si>
+    <t>Plant2</t>
+  </si>
+  <si>
+    <t>plant_owner='3'</t>
+  </si>
+  <si>
+    <t>plant_owner='1'</t>
+  </si>
+  <si>
+    <t>address like '苏州西门子电器有限公司'</t>
+  </si>
+  <si>
+    <t>good request, data retrieved (no schema check, no condition check)</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-1</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-2</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-3</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-4</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-5</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-6</t>
+  </si>
+  <si>
+    <t>iot-connector-differentTablesInOneDb-7</t>
   </si>
 </sst>
 </file>
@@ -643,20 +688,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="1" width="34.15234375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.3828125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.23046875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="12.61328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -697,7 +744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -718,7 +765,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -739,7 +786,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -766,7 +813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
@@ -791,7 +838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -814,7 +861,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -837,7 +884,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -860,7 +907,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -883,7 +930,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -906,7 +953,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -929,7 +976,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
@@ -952,7 +999,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -975,7 +1022,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
@@ -998,7 +1045,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -1021,7 +1068,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
@@ -1044,7 +1091,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -1071,7 +1118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -1098,7 +1145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -1121,7 +1168,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -1146,7 +1193,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
@@ -1171,7 +1218,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
@@ -1196,7 +1243,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
@@ -1223,7 +1270,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
@@ -1250,7 +1297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>63</v>
       </c>
@@ -1277,7 +1324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>64</v>
       </c>
@@ -1304,7 +1351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
@@ -1327,7 +1374,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
@@ -1350,7 +1397,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>67</v>
       </c>
@@ -1373,7 +1420,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>68</v>
       </c>
@@ -1396,7 +1443,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>69</v>
       </c>
@@ -1421,7 +1468,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>70</v>
       </c>
@@ -1446,7 +1493,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
@@ -1471,7 +1518,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1543,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1521,7 +1568,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -1546,7 +1593,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
@@ -1571,7 +1618,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>76</v>
       </c>
@@ -1596,7 +1643,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
@@ -1619,7 +1666,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
@@ -1642,7 +1689,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1665,7 +1712,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>80</v>
       </c>
@@ -1688,7 +1735,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>81</v>
       </c>
@@ -1711,7 +1758,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
@@ -1734,7 +1781,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>83</v>
       </c>
@@ -1757,7 +1804,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>84</v>
       </c>
@@ -1779,6 +1826,139 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
when input parameters pageIndex,pageSize must together order
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B4328B-85A7-4C5C-9719-FB708F4B8295}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E16DBE-D806-4499-9BE6-AB19EB90523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -790,9 +790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2121,7 +2121,9 @@
       <c r="F54" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="H54" s="3">
         <v>1</v>
       </c>
@@ -2412,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE06810-2F00-4AFF-9380-43F6C8BD3078}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add ConnectorOtherInterfacesTests test and iot-connector-configure-test-data.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -8,15 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E16DBE-D806-4499-9BE6-AB19EB90523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48020CB7-6E59-42A1-B6A8-6B274D3605A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
-    <sheet name="saveConnector" sheetId="3" r:id="rId2"/>
-    <sheet name="updateConnector" sheetId="4" r:id="rId3"/>
-    <sheet name="deleteConnector" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
   <si>
     <t>name</t>
   </si>
@@ -328,97 +325,6 @@
   </si>
   <si>
     <t>not exist in entity!</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>Operate success.</t>
-  </si>
-  <si>
-    <t>bad request</t>
-  </si>
-  <si>
-    <t>is duplicated</t>
-  </si>
-  <si>
-    <t>{
-    "connectorName":"",
-    "driverMeta":{
-        "metaName":"JDBC",
-        "metaType":"DRIVER",
-        "metaVersion":"1.0"
-    }
-}</t>
-  </si>
-  <si>
-    <t>connector name cannot be blank;</t>
-  </si>
-  <si>
-    <t>{
-    "connectorName":"TESTCONNECTORREFACTOR_1",
-    "driverMeta":{
-        "metaName":"JDBC",
-        "metaType":"DRIVER",
-        "metaVersion":"1.0"
-    }
-}</t>
-  </si>
-  <si>
-    <t>iot-connector-test-9</t>
-  </si>
-  <si>
-    <t>iot-connector-test-10</t>
-  </si>
-  <si>
-    <t>iot-connector-test-11</t>
-  </si>
-  <si>
-    <t>iot-connector-test-12</t>
-  </si>
-  <si>
-    <t>iot-connector-test-13</t>
-  </si>
-  <si>
-    <t>iot-connector-test-14</t>
-  </si>
-  <si>
-    <t>iot-connector-test-15</t>
-  </si>
-  <si>
-    <t>iot-connector-test-16</t>
-  </si>
-  <si>
-    <t>connectorName</t>
-  </si>
-  <si>
-    <t>TESTCONNECTORREFACTOR_1</t>
-  </si>
-  <si>
-    <t>not found</t>
-  </si>
-  <si>
-    <t>TESTCONNECTORREFACTOR</t>
-  </si>
-  <si>
-    <t>{
-    "connectorName":"TESTCONNECTORREFACTOR",
-    "driverMeta":{
-        "metaName":"JDBC",
-        "metaType":"DRIVER",
-        "metaVersion":"1.0"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "connectorName":"TESTCONNECTORREFACTOR",
-    "driverMeta":{
-        "metaName":"JDBC",
-        "metaType":"DRIVER",
-        "metaVersion":"1.1"
-    }
-}</t>
   </si>
 </sst>
 </file>
@@ -488,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -496,18 +402,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +685,8 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2142,373 +2036,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F420914-9FC2-4EC7-B968-525368C24D09}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="9">
-        <v>106904</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="9">
-        <v>200</v>
-      </c>
-      <c r="E5" s="9">
-        <v>106903</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC440693-2E29-44F5-BCB1-DCA1826A235F}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.6640625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="9">
-        <v>200</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="9">
-        <v>200</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="9">
-        <v>200</v>
-      </c>
-      <c r="F4" s="9">
-        <v>106901</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="9">
-        <v>200</v>
-      </c>
-      <c r="F5" s="9">
-        <v>106901</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE06810-2F00-4AFF-9380-43F6C8BD3078}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="9">
-        <v>200</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="9">
-        <v>200</v>
-      </c>
-      <c r="E3" s="9">
-        <v>106901</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9">
-        <v>200</v>
-      </c>
-      <c r="E4" s="9">
-        <v>106901</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add iot web services read and write case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678B76E7-96BD-4881-8244-50DB416127C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DBBD23-1FF6-4F2B-BF7E-200E7FA8BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
     <sheet name="getDataByConditionForRestfulGet" sheetId="3" r:id="rId2"/>
+    <sheet name="dmlDataInsert" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
   <si>
     <t>name</t>
   </si>
@@ -350,31 +351,85 @@
   </si>
   <si>
     <t>Siid1,SoeEnabled,Siid2,Siid</t>
+  </si>
+  <si>
+    <t>good request, data retrieved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>warehouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertinfo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-webservice-write</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request, data retrieved (no schema check)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request, data retrieved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "warehousewrite":[
+        {
+            "stockItem":[
+                {
+                    "WMS_GUID":"1005",
+                    "BUDAT":"t5"
+                },
+                {
+                    "WMS_GUID":"1007",
+                    "BUDAT":"t7"
+                }
+            ]
+        }
+    ]
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-webservice-read</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -419,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -427,6 +482,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,14 +765,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -732,7 +790,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -773,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -794,7 +852,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -815,7 +873,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -842,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -867,7 +925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -890,7 +948,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -913,7 +971,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -936,7 +994,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -959,7 +1017,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -982,7 +1040,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -1005,7 +1063,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1086,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1051,7 +1109,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1074,7 +1132,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>47</v>
       </c>
@@ -1097,7 +1155,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
@@ -1120,7 +1178,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
@@ -1147,7 +1205,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>57</v>
       </c>
@@ -1174,7 +1232,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
@@ -1197,7 +1255,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
@@ -1222,7 +1280,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1247,7 +1305,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1272,7 +1330,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -1299,7 +1357,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>59</v>
       </c>
@@ -1326,7 +1384,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>60</v>
       </c>
@@ -1353,7 +1411,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -1380,7 +1438,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
@@ -1403,7 +1461,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>63</v>
       </c>
@@ -1426,7 +1484,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>64</v>
       </c>
@@ -1449,7 +1507,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -1472,7 +1530,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -1497,7 +1555,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>67</v>
       </c>
@@ -1522,7 +1580,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1547,7 +1605,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1572,7 +1630,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>70</v>
       </c>
@@ -1597,7 +1655,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -1622,7 +1680,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -1647,7 +1705,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
@@ -1672,7 +1730,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>74</v>
       </c>
@@ -1695,7 +1753,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>75</v>
       </c>
@@ -1718,7 +1776,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
@@ -1741,7 +1799,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -1764,7 +1822,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>78</v>
       </c>
@@ -1787,7 +1845,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>79</v>
       </c>
@@ -1810,12 +1868,12 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1833,7 +1891,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
@@ -1856,7 +1914,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>84</v>
       </c>
@@ -1879,7 +1937,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>92</v>
       </c>
@@ -1902,7 +1960,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>93</v>
       </c>
@@ -1927,7 +1985,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>94</v>
       </c>
@@ -1952,7 +2010,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
@@ -1977,7 +2035,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>96</v>
       </c>
@@ -2002,7 +2060,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>97</v>
       </c>
@@ -2027,12 +2085,12 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2055,6 +2113,20 @@
         <v>0</v>
       </c>
       <c r="M54" s="3"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L55" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2067,11 +2139,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2FB35-017A-40CF-8945-85D992797703}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2083,14 +2155,14 @@
     <col min="8" max="8" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2134,7 +2206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -2164,7 +2236,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>104</v>
       </c>
@@ -2199,4 +2271,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307EFD23-8984-40D2-945A-E144136EC16E}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update test-id=iot-connector-test-2-var2 resposne code and message based on Yongfen latest commit
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92277FE-E25D-4044-B2B2-DC8998343CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E9B4C-2578-4503-8CAD-84A3EB58CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>searchData.name is not valid,reason: must not be blank</t>
   </si>
   <si>
-    <t>The m2 service unavailable: (request M2 failed : no found entity ).</t>
-  </si>
-  <si>
     <t>1=1</t>
   </si>
   <si>
@@ -433,6 +430,10 @@
   <si>
     <t>Unrecognized fields: aa</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>External configuration service is unavailable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -802,9 +803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -820,7 +821,7 @@
     <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
@@ -868,7 +869,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -877,7 +878,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -889,7 +890,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -898,7 +899,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -910,7 +911,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -937,7 +938,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -954,26 +955,26 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>108001</v>
+        <v>106920</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -985,18 +986,18 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1008,18 +1009,18 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1031,18 +1032,18 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1054,18 +1055,18 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1077,18 +1078,18 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1100,18 +1101,18 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1123,18 +1124,18 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1146,7 +1147,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
@@ -1154,10 +1155,10 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1169,7 +1170,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
@@ -1177,10 +1178,10 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1192,7 +1193,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -1200,10 +1201,10 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1215,18 +1216,18 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1237,23 +1238,23 @@
         <v>106107</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1264,12 +1265,12 @@
         <v>106107</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
@@ -1278,10 +1279,10 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1292,7 +1293,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
@@ -1301,10 +1302,10 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
@@ -1317,7 +1318,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1326,10 +1327,10 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
@@ -1342,7 +1343,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1351,10 +1352,10 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3">
@@ -1367,16 +1368,16 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" s="3">
         <v>12321</v>
@@ -1389,21 +1390,21 @@
         <v>106107</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="3">
         <v>12321</v>
@@ -1416,24 +1417,24 @@
         <v>106107</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1443,24 +1444,24 @@
         <v>106107</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1470,12 +1471,12 @@
         <v>106107</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -1484,7 +1485,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3">
@@ -1498,7 +1499,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1507,7 +1508,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3">
@@ -1521,7 +1522,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1530,7 +1531,7 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1544,7 +1545,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1553,7 +1554,7 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1567,7 +1568,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1576,7 +1577,7 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3">
@@ -1592,7 +1593,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1601,7 +1602,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3">
@@ -1617,7 +1618,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1626,7 +1627,7 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3">
@@ -1642,7 +1643,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
@@ -1651,7 +1652,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3">
@@ -1667,7 +1668,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -1676,7 +1677,7 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3">
@@ -1692,7 +1693,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -1701,7 +1702,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3">
@@ -1717,7 +1718,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>5</v>
@@ -1726,7 +1727,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3">
@@ -1742,7 +1743,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>5</v>
@@ -1751,7 +1752,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3">
@@ -1767,7 +1768,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>5</v>
@@ -1776,7 +1777,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
@@ -1790,7 +1791,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
@@ -1799,7 +1800,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3">
@@ -1813,7 +1814,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -1822,7 +1823,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3">
@@ -1836,7 +1837,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -1845,7 +1846,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3">
@@ -1859,7 +1860,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -1868,7 +1869,7 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -1882,7 +1883,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -1891,7 +1892,7 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -1905,16 +1906,16 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -1928,7 +1929,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -1937,7 +1938,7 @@
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -1951,16 +1952,16 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -1974,16 +1975,16 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -1997,18 +1998,18 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2022,18 +2023,18 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2047,18 +2048,18 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2072,10 +2073,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2083,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2097,19 +2098,19 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -2122,19 +2123,19 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H54" s="3">
         <v>1</v>
@@ -2151,13 +2152,13 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L55" s="1">
         <v>0</v>
@@ -2229,7 +2230,7 @@
         <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>14</v>
@@ -2243,7 +2244,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -2252,14 +2253,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L2" s="3">
         <v>200</v>
@@ -2268,12 +2269,12 @@
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -2282,14 +2283,14 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L3" s="3">
         <v>200</v>
@@ -2298,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2312,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307EFD23-8984-40D2-945A-E144136EC16E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2332,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
@@ -2341,18 +2342,18 @@
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -2363,13 +2364,13 @@
     </row>
     <row r="3" spans="1:6" ht="248.4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
         <v>116</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -2378,7 +2379,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify test cases of iot entitymanagement
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCA2120-BFA0-4906-87C8-D8AA85C1DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECE424-D8FD-4743-A9F5-DDD716C97606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>add domain entities for mapping success</t>
+    <t>This entity 12321 is not found in domain</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
@@ -954,7 +954,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>106920</v>
+        <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
add test case for sdl-8227
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECE424-D8FD-4743-A9F5-DDD716C97606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1BC37E-2C08-4297-8F80-B962A243A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
     <sheet name="getDataByConditionForRestfulGet" sheetId="3" r:id="rId2"/>
     <sheet name="dmlDataInsert" sheetId="4" r:id="rId3"/>
+    <sheet name="queryEntityMapToClickhouseTable" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="131">
   <si>
     <t>name</t>
   </si>
@@ -434,35 +435,70 @@
   <si>
     <t>This entity 12321 is not found in domain</t>
   </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClickhouseDriverSensor</t>
+  </si>
+  <si>
+    <t>ClickhouseDriverSensor</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-2</t>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-3</t>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-4</t>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-5</t>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>name='sensorA'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -802,12 +838,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -825,7 +861,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -866,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -887,7 +923,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -908,7 +944,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -935,7 +971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -960,7 +996,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -983,7 +1019,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1006,7 +1042,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1029,7 +1065,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1052,7 +1088,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1075,7 +1111,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1098,7 +1134,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -1121,7 +1157,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -1144,7 +1180,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1167,7 +1203,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
@@ -1190,7 +1226,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1213,7 +1249,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -1240,7 +1276,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -1267,7 +1303,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -1290,7 +1326,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -1315,7 +1351,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -1340,7 +1376,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1365,7 +1401,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
@@ -1392,7 +1428,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
@@ -1419,7 +1455,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1446,7 +1482,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
@@ -1473,7 +1509,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1496,7 +1532,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
@@ -1519,7 +1555,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -1542,7 +1578,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
@@ -1565,7 +1601,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -1590,7 +1626,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
@@ -1615,7 +1651,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
@@ -1640,7 +1676,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1665,7 +1701,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1690,7 +1726,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1715,7 +1751,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
@@ -1740,7 +1776,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
@@ -1765,7 +1801,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -1788,7 +1824,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -1811,7 +1847,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -1834,7 +1870,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
@@ -1857,7 +1893,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -1880,7 +1916,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
@@ -1903,7 +1939,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>79</v>
       </c>
@@ -1926,7 +1962,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
@@ -1949,7 +1985,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>83</v>
       </c>
@@ -1972,7 +2008,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>91</v>
       </c>
@@ -1995,7 +2031,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>92</v>
       </c>
@@ -2020,7 +2056,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
@@ -2045,7 +2081,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>94</v>
       </c>
@@ -2070,7 +2106,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>95</v>
       </c>
@@ -2095,7 +2131,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
@@ -2120,7 +2156,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>97</v>
       </c>
@@ -2149,7 +2185,7 @@
       </c>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>114</v>
       </c>
@@ -2178,9 +2214,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -2197,7 +2233,7 @@
     <col min="15" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2241,7 +2277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2271,7 +2307,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>103</v>
       </c>
@@ -2316,7 +2352,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.21875" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" customWidth="1"/>
@@ -2324,7 +2360,7 @@
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="13.8">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2344,7 +2380,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="108.6" customHeight="1">
+    <row r="2" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -2361,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="259.2">
+    <row r="3" spans="1:6" ht="248.4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2379,6 +2415,152 @@
       </c>
       <c r="F3" t="s">
         <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE1BE47-1B2E-4564-AA59-DF1B57E0B37C}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test cases for SDL-8227
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECE424-D8FD-4743-A9F5-DDD716C97606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99731381-7368-4868-AA8E-AAA7BF9BF05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
     <sheet name="getDataByConditionForRestfulGet" sheetId="3" r:id="rId2"/>
     <sheet name="dmlDataInsert" sheetId="4" r:id="rId3"/>
+    <sheet name="authForRestfulRead" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
   <si>
     <t>name</t>
   </si>
@@ -434,11 +435,207 @@
   <si>
     <t>This entity 12321 is not found in domain</t>
   </si>
+  <si>
+    <t>authInfo</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-1</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserReadWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithBasicAuth</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-2</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>106103</t>
+  </si>
+  <si>
+    <t>sql execution failed</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-3</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:basic)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserReadWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-4</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserReadWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithOauthAuth</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-5</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-6</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:OAUTH)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserReadWithOauthAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-7</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserReadWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithCookieAuth</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-8</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-9</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:Cookie)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserReadWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value3"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-10</t>
+  </si>
+  <si>
+    <t>good request, data retrieved
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserReadWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>UserReadWithTokenAuth</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-11</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is NONE
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>jinzu-restful-read-auth-test-12</t>
+  </si>
+  <si>
+    <t>bad request,authInfo is wrong
+(authType:TOKEN)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserReadWithTokenAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    }
+]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -509,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -519,6 +716,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
@@ -2386,4 +2592,281 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08608831-FC26-436B-96FA-E7725045AD6C}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.6640625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="124.2">
+      <c r="A2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="27.6">
+      <c r="A3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="124.2">
+      <c r="A4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="138">
+      <c r="A5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="27.6">
+      <c r="A6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="138">
+      <c r="A7" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="138">
+      <c r="A8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="27.6">
+      <c r="A9" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="138">
+      <c r="A10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="138">
+      <c r="A11" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="27.6">
+      <c r="A12" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="138">
+      <c r="A13" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add missing case back again
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-connector-test-data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99731381-7368-4868-AA8E-AAA7BF9BF05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EF840C-18A2-4D53-966E-7267986676F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
     <sheet name="getDataByConditionForRestfulGet" sheetId="3" r:id="rId2"/>
     <sheet name="dmlDataInsert" sheetId="4" r:id="rId3"/>
     <sheet name="authForRestfulRead" sheetId="5" r:id="rId4"/>
+    <sheet name="queryEntityMapToClickhouseTable" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="170">
   <si>
     <t>name</t>
   </si>
@@ -628,6 +629,41 @@
     }
 ]</t>
   </si>
+  <si>
+    <t>ClickhouseDriverSensor</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-5</t>
+  </si>
+  <si>
+    <t>ClickhouseDriverSensor</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>name='sensorA'</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-4</t>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-3</t>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-2</t>
+  </si>
+  <si>
+    <t>iot-connector-enittymaptoclickhousetable-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -636,30 +672,30 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1013,7 +1049,7 @@
       <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1031,7 +1067,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1072,7 +1108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1093,7 +1129,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1114,7 +1150,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1166,7 +1202,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1189,7 +1225,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1212,7 +1248,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1235,7 +1271,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1258,7 +1294,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1317,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1304,7 +1340,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
@@ -1327,7 +1363,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -1350,7 +1386,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1373,7 +1409,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
@@ -1396,7 +1432,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1455,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -1446,7 +1482,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -1473,7 +1509,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
@@ -1496,7 +1532,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -1521,7 +1557,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -1546,7 +1582,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1571,7 +1607,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
@@ -1598,7 +1634,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
@@ -1625,7 +1661,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>59</v>
       </c>
@@ -1652,7 +1688,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
@@ -1679,7 +1715,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -1702,7 +1738,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>62</v>
       </c>
@@ -1725,7 +1761,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -1748,7 +1784,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
@@ -1771,7 +1807,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -1796,7 +1832,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
@@ -1821,7 +1857,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>67</v>
       </c>
@@ -1846,7 +1882,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
@@ -1871,7 +1907,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1896,7 +1932,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -1921,7 +1957,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
@@ -1946,7 +1982,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>72</v>
       </c>
@@ -1971,7 +2007,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>73</v>
       </c>
@@ -1994,7 +2030,7 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -2017,7 +2053,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -2040,7 +2076,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
@@ -2063,7 +2099,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -2086,7 +2122,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
@@ -2109,7 +2145,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>79</v>
       </c>
@@ -2132,7 +2168,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
@@ -2155,7 +2191,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>83</v>
       </c>
@@ -2178,7 +2214,7 @@
       </c>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>91</v>
       </c>
@@ -2201,7 +2237,7 @@
       </c>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>92</v>
       </c>
@@ -2226,7 +2262,7 @@
       </c>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
@@ -2251,7 +2287,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>94</v>
       </c>
@@ -2276,7 +2312,7 @@
       </c>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>95</v>
       </c>
@@ -2301,7 +2337,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>96</v>
       </c>
@@ -2326,7 +2362,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>97</v>
       </c>
@@ -2355,7 +2391,7 @@
       </c>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>114</v>
       </c>
@@ -2384,7 +2420,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2403,7 +2439,7 @@
     <col min="15" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2447,7 +2483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>99</v>
       </c>
@@ -2477,7 +2513,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>103</v>
       </c>
@@ -2522,7 +2558,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.21875" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" customWidth="1"/>
@@ -2530,7 +2566,7 @@
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="13.8">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2550,7 +2586,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="108.6" customHeight="1">
+    <row r="2" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -2567,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="259.2">
+    <row r="3" spans="1:6" ht="248.4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2598,11 +2634,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08608831-FC26-436B-96FA-E7725045AD6C}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.21875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="9" bestFit="1" customWidth="1"/>
@@ -2614,7 +2650,7 @@
     <col min="8" max="16384" width="12.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -2637,7 +2673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="124.2">
+    <row r="2" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>122</v>
       </c>
@@ -2654,7 +2690,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="27.6">
+    <row r="3" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>126</v>
       </c>
@@ -2673,7 +2709,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="124.2">
+    <row r="4" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>130</v>
       </c>
@@ -2694,7 +2730,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="138">
+    <row r="5" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>133</v>
       </c>
@@ -2711,7 +2747,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="27.6">
+    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>137</v>
       </c>
@@ -2730,7 +2766,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="138">
+    <row r="7" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>139</v>
       </c>
@@ -2751,7 +2787,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="138">
+    <row r="8" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>142</v>
       </c>
@@ -2768,7 +2804,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6">
+    <row r="9" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>146</v>
       </c>
@@ -2787,7 +2823,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="138">
+    <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>148</v>
       </c>
@@ -2808,7 +2844,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="138">
+    <row r="11" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>151</v>
       </c>
@@ -2825,7 +2861,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="27.6">
+    <row r="12" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>155</v>
       </c>
@@ -2844,7 +2880,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="138">
+    <row r="13" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>157</v>
       </c>
@@ -2866,6 +2902,153 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B82A7AB-E4EA-43BB-BB01-3A11291E21A8}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>